<commit_message>
upload page designed, load to temp table
</commit_message>
<xml_diff>
--- a/src/App/PolioDbBundle/Controller/Render/Book1.xlsx
+++ b/src/App/PolioDbBundle/Controller/Render/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\poliodb\src\App\PolioDbBundle\Controller\Render\"/>
@@ -54,7 +54,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -66,6 +66,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -92,9 +100,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -376,23 +385,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="K17" sqref="F1:K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" s="2"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -400,7 +411,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -408,7 +419,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -420,8 +431,8 @@
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1"/>
     <hyperlink ref="B2" r:id="rId2"/>
-    <hyperlink ref="B3" r:id="rId3"/>
-    <hyperlink ref="B4" r:id="rId4"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B3" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>